<commit_message>
update REST API guide
</commit_message>
<xml_diff>
--- a/REST API guide.xlsx
+++ b/REST API guide.xlsx
@@ -760,108 +760,129 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -870,27 +891,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1199,8 +1199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1224,65 +1224,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="20"/>
-      <c r="B1" s="21" t="s">
+      <c r="A1" s="57"/>
+      <c r="B1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A2" s="20"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="22" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="21" t="s">
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21" t="s">
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21" t="s">
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
     </row>
     <row r="3" spans="1:19" s="6" customFormat="1">
-      <c r="A3" s="20"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="25"/>
+      <c r="A3" s="57"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="54"/>
       <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
@@ -1331,10 +1331,10 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="30">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="53" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1346,7 +1346,7 @@
       <c r="E4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="41" t="s">
+      <c r="F4" s="31" t="s">
         <v>48</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -1358,7 +1358,7 @@
       <c r="I4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="29" t="s">
+      <c r="J4" s="19" t="s">
         <v>44</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -1374,21 +1374,21 @@
       <c r="S4" s="12"/>
     </row>
     <row r="5" spans="1:19" ht="30">
-      <c r="A5" s="54"/>
-      <c r="B5" s="23"/>
+      <c r="A5" s="61"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="43" t="s">
+      <c r="F5" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="26" t="s">
         <v>20</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -1397,7 +1397,7 @@
       <c r="I5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="30" t="s">
+      <c r="J5" s="20" t="s">
         <v>45</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -1413,21 +1413,21 @@
       <c r="S5" s="10"/>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="54"/>
-      <c r="B6" s="23"/>
+      <c r="A6" s="61"/>
+      <c r="B6" s="58"/>
       <c r="C6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="44" t="s">
+      <c r="F6" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="27" t="s">
         <v>20</v>
       </c>
       <c r="H6" s="8" t="s">
@@ -1436,7 +1436,7 @@
       <c r="I6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="31" t="s">
+      <c r="J6" s="21" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="2" t="s">
@@ -1452,15 +1452,15 @@
       <c r="S6" s="13"/>
     </row>
     <row r="7" spans="1:19" ht="28.35" customHeight="1">
-      <c r="A7" s="54"/>
-      <c r="B7" s="24"/>
+      <c r="A7" s="61"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D7" s="11"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="38"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="28"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
@@ -1483,8 +1483,8 @@
       </c>
     </row>
     <row r="8" spans="1:19">
-      <c r="A8" s="54"/>
-      <c r="B8" s="22" t="s">
+      <c r="A8" s="61"/>
+      <c r="B8" s="53" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1493,13 +1493,13 @@
       <c r="D8" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="46" t="s">
+      <c r="F8" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="39" t="s">
+      <c r="G8" s="29" t="s">
         <v>33</v>
       </c>
       <c r="H8" s="15"/>
@@ -1516,21 +1516,21 @@
       <c r="S8" s="16"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="A9" s="54"/>
-      <c r="B9" s="23"/>
+      <c r="A9" s="61"/>
+      <c r="B9" s="58"/>
       <c r="C9" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="47" t="s">
+      <c r="F9" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="40" t="s">
+      <c r="G9" s="30" t="s">
         <v>33</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -1539,7 +1539,7 @@
       <c r="I9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="J9" s="30" t="s">
+      <c r="J9" s="20" t="s">
         <v>56</v>
       </c>
       <c r="K9" s="2" t="s">
@@ -1555,14 +1555,14 @@
       <c r="S9" s="11"/>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="54"/>
-      <c r="B10" s="23"/>
+      <c r="A10" s="61"/>
+      <c r="B10" s="58"/>
       <c r="C10" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
-      <c r="F10" s="42"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="11"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
@@ -1578,8 +1578,8 @@
       <c r="S10" s="11"/>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="54"/>
-      <c r="B11" s="25"/>
+      <c r="A11" s="61"/>
+      <c r="B11" s="54"/>
       <c r="C11" s="4" t="s">
         <v>31</v>
       </c>
@@ -1601,8 +1601,8 @@
       <c r="S11" s="11"/>
     </row>
     <row r="12" spans="1:19" ht="30">
-      <c r="A12" s="54"/>
-      <c r="B12" s="22" t="s">
+      <c r="A12" s="61"/>
+      <c r="B12" s="53" t="s">
         <v>57</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -1634,8 +1634,8 @@
       <c r="S12" s="11"/>
     </row>
     <row r="13" spans="1:19" ht="30">
-      <c r="A13" s="54"/>
-      <c r="B13" s="23"/>
+      <c r="A13" s="61"/>
+      <c r="B13" s="58"/>
       <c r="C13" s="4" t="s">
         <v>58</v>
       </c>
@@ -1657,7 +1657,7 @@
       <c r="I13" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="J13" s="50" t="s">
+      <c r="J13" s="40" t="s">
         <v>69</v>
       </c>
       <c r="K13" s="4" t="s">
@@ -1673,7 +1673,7 @@
       <c r="Q13" t="s">
         <v>71</v>
       </c>
-      <c r="R13" s="50" t="s">
+      <c r="R13" s="40" t="s">
         <v>65</v>
       </c>
       <c r="S13" s="4" t="s">
@@ -1681,9 +1681,9 @@
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="54"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="49" t="s">
+      <c r="A14" s="61"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="39" t="s">
         <v>59</v>
       </c>
       <c r="D14" s="11"/>
@@ -1704,12 +1704,12 @@
       <c r="S14" s="11"/>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="55"/>
+      <c r="A15" s="62"/>
       <c r="B15" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="46"/>
-      <c r="D15" s="40"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="30"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -1727,20 +1727,20 @@
       <c r="S15" s="11"/>
     </row>
     <row r="16" spans="1:19">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="55" t="s">
         <v>76</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="42"/>
+      <c r="C16" s="32"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
-      <c r="J16" s="62"/>
+      <c r="J16" s="45"/>
       <c r="K16" s="11"/>
       <c r="L16" s="4" t="s">
         <v>77</v>
@@ -1748,7 +1748,7 @@
       <c r="M16" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="N16" s="50" t="s">
+      <c r="N16" s="40" t="s">
         <v>79</v>
       </c>
       <c r="O16" s="4" t="s">
@@ -1760,7 +1760,7 @@
       <c r="S16" s="10"/>
     </row>
     <row r="17" spans="1:19">
-      <c r="A17" s="19"/>
+      <c r="A17" s="55"/>
       <c r="B17" s="5" t="s">
         <v>7</v>
       </c>
@@ -1770,13 +1770,13 @@
       <c r="D17" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="35" t="s">
+      <c r="E17" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="46" t="s">
+      <c r="F17" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="39" t="s">
+      <c r="G17" s="29" t="s">
         <v>20</v>
       </c>
       <c r="H17" s="10"/>
@@ -1793,7 +1793,7 @@
       <c r="S17" s="10"/>
     </row>
     <row r="18" spans="1:19">
-      <c r="A18" s="19"/>
+      <c r="A18" s="55"/>
       <c r="B18" s="17" t="s">
         <v>8</v>
       </c>
@@ -1816,11 +1816,11 @@
       <c r="S18" s="10"/>
     </row>
     <row r="19" spans="1:19">
-      <c r="A19" s="51"/>
-      <c r="B19" s="52" t="s">
+      <c r="A19" s="56"/>
+      <c r="B19" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="40"/>
+      <c r="C19" s="30"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -1839,19 +1839,19 @@
       <c r="S19" s="2"/>
     </row>
     <row r="21" spans="1:19" ht="30">
-      <c r="A21" s="57" t="s">
+      <c r="A21" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="B21" s="52" t="s">
+      <c r="B21" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="58" t="s">
+      <c r="C21" s="43" t="s">
         <v>85</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="E21" s="59" t="s">
+      <c r="E21" s="44" t="s">
         <v>86</v>
       </c>
       <c r="F21" s="9" t="s">
@@ -1862,22 +1862,22 @@
       <c r="B22"/>
     </row>
     <row r="23" spans="1:19" ht="20.25">
-      <c r="B23" s="60" t="s">
+      <c r="B23" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="60"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="60"/>
-      <c r="K23" s="60"/>
-      <c r="L23" s="60"/>
-      <c r="M23" s="60"/>
-      <c r="N23" s="60"/>
-      <c r="O23" s="60"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="48"/>
+      <c r="L23" s="48"/>
+      <c r="M23" s="48"/>
+      <c r="N23" s="48"/>
+      <c r="O23" s="48"/>
     </row>
     <row r="24" spans="1:19">
       <c r="B24"/>
@@ -1886,106 +1886,113 @@
       <c r="A25" t="s">
         <v>81</v>
       </c>
-      <c r="B25" s="56" t="s">
+      <c r="B25" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="56"/>
-      <c r="J25" s="56"/>
-      <c r="K25" s="56"/>
-      <c r="L25" s="56"/>
-      <c r="M25" s="56"/>
-      <c r="N25" s="56"/>
-      <c r="O25" s="56"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="46"/>
+      <c r="N25" s="46"/>
+      <c r="O25" s="46"/>
     </row>
     <row r="26" spans="1:19" ht="129" customHeight="1">
-      <c r="B26" s="56" t="s">
+      <c r="B26" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="56"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="56"/>
-      <c r="H26" s="56"/>
-      <c r="I26" s="56"/>
-      <c r="J26" s="56"/>
-      <c r="K26" s="56"/>
-      <c r="L26" s="56"/>
-      <c r="M26" s="56"/>
-      <c r="N26" s="56"/>
-      <c r="O26" s="56"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="46"/>
+      <c r="N26" s="46"/>
+      <c r="O26" s="46"/>
     </row>
     <row r="27" spans="1:19" ht="20.25">
-      <c r="B27" s="61" t="s">
+      <c r="B27" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="C27" s="61"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="61"/>
-      <c r="J27" s="61"/>
-      <c r="K27" s="61"/>
-      <c r="L27" s="61"/>
-      <c r="M27" s="61"/>
-      <c r="N27" s="61"/>
-      <c r="O27" s="61"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="47"/>
+      <c r="J27" s="47"/>
+      <c r="K27" s="47"/>
+      <c r="L27" s="47"/>
+      <c r="M27" s="47"/>
+      <c r="N27" s="47"/>
+      <c r="O27" s="47"/>
     </row>
     <row r="28" spans="1:19">
-      <c r="B28" s="48"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="48"/>
-      <c r="I28" s="48"/>
-      <c r="J28" s="48"/>
-      <c r="K28" s="48"/>
-      <c r="L28" s="48"/>
-      <c r="M28" s="48"/>
-      <c r="N28" s="48"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="38"/>
+      <c r="M28" s="38"/>
+      <c r="N28" s="38"/>
     </row>
     <row r="29" spans="1:19">
-      <c r="B29" s="48"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="48"/>
-      <c r="H29" s="48"/>
-      <c r="I29" s="48"/>
-      <c r="J29" s="48"/>
-      <c r="K29" s="48"/>
-      <c r="L29" s="48"/>
-      <c r="M29" s="48"/>
-      <c r="N29" s="48"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="38"/>
+      <c r="M29" s="38"/>
+      <c r="N29" s="38"/>
     </row>
     <row r="30" spans="1:19">
-      <c r="B30" s="48"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="48"/>
-      <c r="K30" s="48"/>
-      <c r="L30" s="48"/>
-      <c r="M30" s="48"/>
-      <c r="N30" s="48"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="38"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="38"/>
+      <c r="N30" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="A4:A15"/>
     <mergeCell ref="B25:O25"/>
     <mergeCell ref="B26:O26"/>
     <mergeCell ref="B27:O27"/>
@@ -1996,13 +2003,6 @@
     <mergeCell ref="P2:S2"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="A4:A15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0" right="0" top="0.39370000000000011" bottom="0.39370000000000011" header="0" footer="0"/>

</xml_diff>

<commit_message>
revise REST API GUIDE
</commit_message>
<xml_diff>
--- a/REST API guide.xlsx
+++ b/REST API guide.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="110">
   <si>
     <t>Controller</t>
   </si>
@@ -82,18 +82,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>user/info/[params]</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>user/msg/[params]</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>array</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Function</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -138,10 +126,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>array</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>boolean</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -162,10 +146,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>location/msg/[params]</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>store location msg</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -174,10 +154,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>boolean</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Param available</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -269,10 +245,6 @@
     <t>user_followed</t>
   </si>
   <si>
-    <t>boolean</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>follow a person</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -314,10 +286,6 @@
   </si>
   <si>
     <t>register</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>boolean</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -408,11 +376,87 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>user/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>boolean</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>user/</t>
+    <t>user/info/[params pair]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>error</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>401:unthorized200:success</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>email,name,gender,faculty,major,status,hobbies</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>json array: email,name,gender,faculty,major,hobbies,status,profile</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>json array: email,name,gender,faculty,major,hobbies,statusprofile</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>error</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>param</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>401:unthorized200:success</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>json array: location_id,name,description,geometry</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>json array: email,timestamp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>200:success</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>error</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>user/info/[params pair]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>user/msg/[params pair]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>location/msg/[params pairs]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>json array: geometry timestamp, email</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>json array: content,user_to,user_from,timestamp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>json array: email,content,location_id,location_name</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -719,22 +763,20 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
       <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
+      <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -756,7 +798,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -835,25 +877,13 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -898,8 +928,44 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -910,9 +976,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -922,41 +985,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1263,10 +1350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1275,132 +1362,144 @@
     <col min="2" max="2" width="11.42578125" style="6" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="6" width="22.140625" customWidth="1"/>
-    <col min="7" max="7" width="7" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" customWidth="1"/>
-    <col min="13" max="14" width="11.5703125" customWidth="1"/>
-    <col min="15" max="15" width="12" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" customWidth="1"/>
-    <col min="17" max="18" width="20.7109375" customWidth="1"/>
-    <col min="19" max="19" width="8.7109375" customWidth="1"/>
+    <col min="5" max="7" width="22.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="12" width="22.140625" customWidth="1"/>
+    <col min="13" max="13" width="15" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="15" max="16" width="11.5703125" customWidth="1"/>
+    <col min="17" max="17" width="12" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" customWidth="1"/>
+    <col min="19" max="20" width="20.7109375" customWidth="1"/>
+    <col min="21" max="21" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" s="62"/>
-      <c r="B1" s="51" t="s">
+    <row r="1" spans="1:21">
+      <c r="A1" s="47"/>
+      <c r="B1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-    </row>
-    <row r="2" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A2" s="62"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="55" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="52" t="s">
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="48"/>
+      <c r="U1" s="48"/>
+    </row>
+    <row r="2" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A2" s="47"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="51" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51" t="s">
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51" t="s">
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-    </row>
-    <row r="3" spans="1:19" s="6" customFormat="1">
-      <c r="A3" s="62"/>
-      <c r="B3" s="51"/>
-      <c r="C3" s="56"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
+      <c r="U2" s="48"/>
+    </row>
+    <row r="3" spans="1:21" s="6" customFormat="1">
+      <c r="A3" s="47"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="52"/>
       <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="75" t="s">
+        <v>97</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="K3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5" t="s">
+      <c r="P3" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="R3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="S3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="S3" s="5" t="s">
+      <c r="T3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="U3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="30">
-      <c r="A4" s="64" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" s="55" t="s">
+    <row r="4" spans="1:21" ht="60">
+      <c r="A4" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="49" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1409,78 +1508,90 @@
       <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="31" t="s">
-        <v>47</v>
+      <c r="E4" s="80" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" s="78" t="s">
+        <v>41</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
+      <c r="K4" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="N4" s="10"/>
       <c r="O4" s="10"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="11"/>
       <c r="S4" s="12"/>
-    </row>
-    <row r="5" spans="1:19" ht="30">
-      <c r="A5" s="65"/>
-      <c r="B5" s="63"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+    </row>
+    <row r="5" spans="1:21" ht="45">
+      <c r="A5" s="54"/>
+      <c r="B5" s="50"/>
       <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
+      <c r="K5" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
       <c r="P5" s="10"/>
       <c r="Q5" s="10"/>
       <c r="R5" s="10"/>
       <c r="S5" s="10"/>
-    </row>
-    <row r="6" spans="1:19">
-      <c r="A6" s="65"/>
-      <c r="B6" s="63"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+    </row>
+    <row r="6" spans="1:21" ht="30">
+      <c r="A6" s="54"/>
+      <c r="B6" s="50"/>
       <c r="C6" s="7" t="s">
         <v>15</v>
       </c>
@@ -1488,205 +1599,231 @@
         <v>17</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>28</v>
+        <v>46</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="I6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
+      <c r="M6" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="N6" s="13"/>
       <c r="O6" s="13"/>
       <c r="P6" s="13"/>
       <c r="Q6" s="13"/>
       <c r="R6" s="13"/>
       <c r="S6" s="13"/>
-    </row>
-    <row r="7" spans="1:19" ht="28.35" customHeight="1">
-      <c r="A7" s="65"/>
-      <c r="B7" s="58"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+    </row>
+    <row r="7" spans="1:21" ht="28.35" customHeight="1">
+      <c r="A7" s="54"/>
+      <c r="B7" s="51"/>
       <c r="C7" s="4" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="24"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="F7" s="31"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="26"/>
       <c r="I7" s="9" t="s">
-        <v>90</v>
+        <v>27</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
+        <v>43</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="N7" s="14"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
       <c r="Q7" s="10"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
-    </row>
-    <row r="8" spans="1:19">
-      <c r="A8" s="65"/>
-      <c r="B8" s="55" t="s">
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+    </row>
+    <row r="8" spans="1:21" ht="45">
+      <c r="A8" s="54"/>
+      <c r="B8" s="49" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="15"/>
+        <v>45</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
       <c r="N8" s="16"/>
       <c r="O8" s="16"/>
       <c r="P8" s="16"/>
       <c r="Q8" s="16"/>
       <c r="R8" s="16"/>
       <c r="S8" s="16"/>
-    </row>
-    <row r="9" spans="1:19">
-      <c r="A9" s="65"/>
-      <c r="B9" s="63"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
+    </row>
+    <row r="9" spans="1:21" ht="45">
+      <c r="A9" s="54"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J9" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
+      <c r="K9" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="N9" s="11"/>
       <c r="O9" s="11"/>
       <c r="P9" s="11"/>
       <c r="Q9" s="11"/>
       <c r="R9" s="11"/>
       <c r="S9" s="11"/>
-    </row>
-    <row r="10" spans="1:19">
-      <c r="A10" s="65"/>
-      <c r="B10" s="63"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" s="54"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="10"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="76"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
       <c r="N10" s="11"/>
       <c r="O10" s="11"/>
       <c r="P10" s="11"/>
       <c r="Q10" s="11"/>
       <c r="R10" s="11"/>
       <c r="S10" s="11"/>
-    </row>
-    <row r="11" spans="1:19">
-      <c r="A11" s="65"/>
-      <c r="B11" s="56"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" s="54"/>
+      <c r="B11" s="52"/>
       <c r="C11" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="10"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="76"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
       <c r="N11" s="11"/>
       <c r="O11" s="11"/>
       <c r="P11" s="11"/>
       <c r="Q11" s="11"/>
       <c r="R11" s="11"/>
       <c r="S11" s="11"/>
-    </row>
-    <row r="12" spans="1:19" ht="30">
-      <c r="A12" s="65"/>
-      <c r="B12" s="55" t="s">
-        <v>56</v>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+    </row>
+    <row r="12" spans="1:21" ht="30">
+      <c r="A12" s="54"/>
+      <c r="B12" s="49" t="s">
+        <v>50</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="11"/>
+        <v>53</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
@@ -1698,65 +1835,73 @@
       <c r="Q12" s="11"/>
       <c r="R12" s="11"/>
       <c r="S12" s="11"/>
-    </row>
-    <row r="13" spans="1:19" ht="30">
-      <c r="A13" s="65"/>
-      <c r="B13" s="63"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+    </row>
+    <row r="13" spans="1:21" ht="30">
+      <c r="A13" s="54"/>
+      <c r="B13" s="50"/>
       <c r="C13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="J13" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="J13" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
+      <c r="K13" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="N13" s="11"/>
       <c r="O13" s="11"/>
-      <c r="P13" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>70</v>
-      </c>
-      <c r="R13" s="40" t="s">
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="S13" t="s">
+        <v>63</v>
+      </c>
+      <c r="T13" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="U13" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="S13" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19">
-      <c r="A14" s="65"/>
-      <c r="B14" s="56"/>
-      <c r="C14" s="39" t="s">
-        <v>58</v>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" s="54"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="35" t="s">
+        <v>52</v>
       </c>
       <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="76"/>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
@@ -1768,98 +1913,110 @@
       <c r="Q14" s="11"/>
       <c r="R14" s="11"/>
       <c r="S14" s="11"/>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="A15" s="66"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" s="55"/>
       <c r="B15" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+        <v>66</v>
+      </c>
+      <c r="C15" s="32"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="27"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
       <c r="N15" s="11"/>
       <c r="O15" s="11"/>
       <c r="P15" s="11"/>
       <c r="Q15" s="11"/>
       <c r="R15" s="11"/>
       <c r="S15" s="11"/>
-    </row>
-    <row r="16" spans="1:19">
-      <c r="A16" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" s="57" t="s">
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="A16" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="46"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="4" t="s">
-        <v>93</v>
-      </c>
+      <c r="C16" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="42"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="79"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="42"/>
       <c r="I16" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="J16" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
+        <v>85</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="K16" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="N16" s="11"/>
       <c r="O16" s="11"/>
       <c r="P16" s="11"/>
       <c r="Q16" s="11"/>
       <c r="R16" s="11"/>
       <c r="S16" s="11"/>
-    </row>
-    <row r="17" spans="1:19" ht="30">
-      <c r="A17" s="60"/>
-      <c r="B17" s="58"/>
-      <c r="C17" s="45" t="s">
-        <v>91</v>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+    </row>
+    <row r="17" spans="1:21" ht="30">
+      <c r="A17" s="45"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="41" t="s">
+        <v>83</v>
       </c>
       <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="4" t="s">
-        <v>76</v>
-      </c>
+      <c r="E17" s="24"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="76"/>
       <c r="I17" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="J17" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
+        <v>69</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K17" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="N17" s="11"/>
       <c r="O17" s="11"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
       <c r="R17" s="10"/>
       <c r="S17" s="10"/>
-    </row>
-    <row r="18" spans="1:19">
-      <c r="A18" s="60"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+    </row>
+    <row r="18" spans="1:21" ht="45">
+      <c r="A18" s="45"/>
       <c r="B18" s="5" t="s">
         <v>7</v>
       </c>
@@ -1867,18 +2024,20 @@
         <v>10</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="F18" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="G18" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="10"/>
+        <v>45</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
@@ -1890,18 +2049,20 @@
       <c r="Q18" s="10"/>
       <c r="R18" s="10"/>
       <c r="S18" s="10"/>
-    </row>
-    <row r="19" spans="1:19">
-      <c r="A19" s="60"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+    </row>
+    <row r="19" spans="1:21">
+      <c r="A19" s="45"/>
       <c r="B19" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="10"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="76"/>
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
@@ -1913,18 +2074,20 @@
       <c r="Q19" s="10"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
-    </row>
-    <row r="20" spans="1:19">
-      <c r="A20" s="61"/>
-      <c r="B20" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="30"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+    </row>
+    <row r="20" spans="1:21">
+      <c r="A20" s="46"/>
+      <c r="B20" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="27"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="2"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="27"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
@@ -1936,155 +2099,183 @@
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
-    </row>
-    <row r="22" spans="1:19" ht="30">
-      <c r="A22" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="B22" s="41" t="s">
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+    </row>
+    <row r="22" spans="1:21" ht="30">
+      <c r="A22" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="73"/>
+    </row>
+    <row r="23" spans="1:21">
+      <c r="B23"/>
+    </row>
+    <row r="24" spans="1:21" ht="20.25">
+      <c r="B24" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="58"/>
+      <c r="J24" s="58"/>
+      <c r="K24" s="58"/>
+      <c r="L24" s="58"/>
+      <c r="M24" s="58"/>
+      <c r="N24" s="58"/>
+      <c r="O24" s="58"/>
+      <c r="P24" s="58"/>
+      <c r="Q24" s="58"/>
+    </row>
+    <row r="25" spans="1:21">
+      <c r="B25"/>
+    </row>
+    <row r="26" spans="1:21" ht="39" customHeight="1">
+      <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="56"/>
+      <c r="H26" s="56"/>
+      <c r="I26" s="56"/>
+      <c r="J26" s="56"/>
+      <c r="K26" s="56"/>
+      <c r="L26" s="56"/>
+      <c r="M26" s="56"/>
+      <c r="N26" s="56"/>
+      <c r="O26" s="56"/>
+      <c r="P26" s="56"/>
+      <c r="Q26" s="56"/>
+    </row>
+    <row r="27" spans="1:21" ht="129" customHeight="1">
+      <c r="B27" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="56"/>
+      <c r="J27" s="56"/>
+      <c r="K27" s="56"/>
+      <c r="L27" s="56"/>
+      <c r="M27" s="56"/>
+      <c r="N27" s="56"/>
+      <c r="O27" s="56"/>
+      <c r="P27" s="56"/>
+      <c r="Q27" s="56"/>
+    </row>
+    <row r="28" spans="1:21" ht="20.25">
+      <c r="B28" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="43" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" s="44" t="s">
-        <v>82</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19">
-      <c r="B23"/>
-    </row>
-    <row r="24" spans="1:19" ht="20.25">
-      <c r="B24" s="50" t="s">
-        <v>86</v>
-      </c>
-      <c r="C24" s="50"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="50"/>
-      <c r="H24" s="50"/>
-      <c r="I24" s="50"/>
-      <c r="J24" s="50"/>
-      <c r="K24" s="50"/>
-      <c r="L24" s="50"/>
-      <c r="M24" s="50"/>
-      <c r="N24" s="50"/>
-      <c r="O24" s="50"/>
-    </row>
-    <row r="25" spans="1:19">
-      <c r="B25"/>
-    </row>
-    <row r="26" spans="1:19" ht="39" customHeight="1">
-      <c r="A26" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" s="48" t="s">
-        <v>85</v>
-      </c>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="48"/>
-      <c r="I26" s="48"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="48"/>
-      <c r="L26" s="48"/>
-      <c r="M26" s="48"/>
-      <c r="N26" s="48"/>
-      <c r="O26" s="48"/>
-    </row>
-    <row r="27" spans="1:19" ht="129" customHeight="1">
-      <c r="B27" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="48"/>
-      <c r="I27" s="48"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="48"/>
-      <c r="L27" s="48"/>
-      <c r="M27" s="48"/>
-      <c r="N27" s="48"/>
-      <c r="O27" s="48"/>
-    </row>
-    <row r="28" spans="1:19" ht="20.25">
-      <c r="B28" s="49" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="49"/>
-      <c r="K28" s="49"/>
-      <c r="L28" s="49"/>
-      <c r="M28" s="49"/>
-      <c r="N28" s="49"/>
-      <c r="O28" s="49"/>
-    </row>
-    <row r="29" spans="1:19">
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
-      <c r="K29" s="38"/>
-      <c r="L29" s="38"/>
-      <c r="M29" s="38"/>
-      <c r="N29" s="38"/>
-    </row>
-    <row r="30" spans="1:19">
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="38"/>
-      <c r="L30" s="38"/>
-      <c r="M30" s="38"/>
-      <c r="N30" s="38"/>
-    </row>
-    <row r="31" spans="1:19">
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="38"/>
-      <c r="K31" s="38"/>
-      <c r="L31" s="38"/>
-      <c r="M31" s="38"/>
-      <c r="N31" s="38"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="57"/>
+      <c r="J28" s="57"/>
+      <c r="K28" s="57"/>
+      <c r="L28" s="57"/>
+      <c r="M28" s="57"/>
+      <c r="N28" s="57"/>
+      <c r="O28" s="57"/>
+      <c r="P28" s="57"/>
+      <c r="Q28" s="57"/>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="34"/>
+      <c r="L29" s="34"/>
+      <c r="M29" s="34"/>
+      <c r="N29" s="34"/>
+      <c r="O29" s="34"/>
+      <c r="P29" s="34"/>
+    </row>
+    <row r="30" spans="1:21">
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="34"/>
+      <c r="L30" s="34"/>
+      <c r="M30" s="34"/>
+      <c r="N30" s="34"/>
+      <c r="O30" s="34"/>
+      <c r="P30" s="34"/>
+    </row>
+    <row r="31" spans="1:21">
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="34"/>
+      <c r="L31" s="34"/>
+      <c r="M31" s="34"/>
+      <c r="N31" s="34"/>
+      <c r="O31" s="34"/>
+      <c r="P31" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B26:Q26"/>
+    <mergeCell ref="B27:Q27"/>
+    <mergeCell ref="B28:Q28"/>
+    <mergeCell ref="B24:Q24"/>
+    <mergeCell ref="C1:U1"/>
+    <mergeCell ref="I2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B16:B17"/>
     <mergeCell ref="A16:A20"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
@@ -2092,17 +2283,6 @@
     <mergeCell ref="B8:B11"/>
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="A4:A15"/>
-    <mergeCell ref="B26:O26"/>
-    <mergeCell ref="B27:O27"/>
-    <mergeCell ref="B28:O28"/>
-    <mergeCell ref="B24:O24"/>
-    <mergeCell ref="C1:S1"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B16:B17"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0" right="0" top="0.39370000000000011" bottom="0.39370000000000011" header="0" footer="0"/>
@@ -2116,15 +2296,161 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="8" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="69"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="66" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="66" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="66" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="66" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="66" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="66" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="60">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="60">
+      <c r="A4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="68" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="33" customHeight="1">
+      <c r="A6" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="72" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="71" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0" right="0" top="0.39370000000000011" bottom="0.39370000000000011" header="0" footer="0"/>
   <headerFooter>

</xml_diff>